<commit_message>
minor updates to column titles in data files for easier processing
</commit_message>
<xml_diff>
--- a/data/all_data.xlsx
+++ b/data/all_data.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sydnidee/Library/CloudStorage/OneDrive-Personal/School/YEAR 5/DATA VIZ/Project 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troyspringmeadows/tv-time/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D88713E-6CA5-AE43-BB05-BA5352C95492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6182D2-92A8-8E46-9EDF-3997C3002FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{D6E1F5BB-695F-B243-9E7C-4B6C1748E0AB}"/>
+    <workbookView xWindow="-32680" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{D6E1F5BB-695F-B243-9E7C-4B6C1748E0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -71,57 +70,6 @@
     <t>Character</t>
   </si>
   <si>
-    <t>Total Lines</t>
-  </si>
-  <si>
-    <t>S1 Lines</t>
-  </si>
-  <si>
-    <t>S2 Lines</t>
-  </si>
-  <si>
-    <t>S3 Lines</t>
-  </si>
-  <si>
-    <t>S4 Lines</t>
-  </si>
-  <si>
-    <t>S5 Lines</t>
-  </si>
-  <si>
-    <t>S6 Lines</t>
-  </si>
-  <si>
-    <t>S7 Lines</t>
-  </si>
-  <si>
-    <t>Top 1 Line</t>
-  </si>
-  <si>
-    <t>Top 2 Line</t>
-  </si>
-  <si>
-    <t>Top 3 Line</t>
-  </si>
-  <si>
-    <t>Top 1 Word</t>
-  </si>
-  <si>
-    <t>Top 2 Word</t>
-  </si>
-  <si>
-    <t>Top 3 Word</t>
-  </si>
-  <si>
-    <t>Top 1 Line Count</t>
-  </si>
-  <si>
-    <t>Top 2 Line Count</t>
-  </si>
-  <si>
-    <t>Top 3 Line Count</t>
-  </si>
-  <si>
     <t>okay</t>
   </si>
   <si>
@@ -215,81 +163,12 @@
     <t>ugh</t>
   </si>
   <si>
-    <t>Top 1 Word Count</t>
-  </si>
-  <si>
-    <t>Top 2 Word Count</t>
-  </si>
-  <si>
-    <t>Top 3 Word Count</t>
-  </si>
-  <si>
-    <t>Top 4 Word</t>
-  </si>
-  <si>
-    <t>Top 4 Word Count</t>
-  </si>
-  <si>
-    <t>Top 5 Word</t>
-  </si>
-  <si>
-    <t>Top 5 Word Count</t>
-  </si>
-  <si>
-    <t>Top 6 Word</t>
-  </si>
-  <si>
-    <t>Top 6 Word Count</t>
-  </si>
-  <si>
-    <t>Top 7 Word</t>
-  </si>
-  <si>
-    <t>Top 7 Word Count</t>
-  </si>
-  <si>
-    <t>Top 8 Word</t>
-  </si>
-  <si>
-    <t>Top 8 Word Count</t>
-  </si>
-  <si>
-    <t>Top 9 Word</t>
-  </si>
-  <si>
-    <t>Top 9 Word Count</t>
-  </si>
-  <si>
-    <t>Top 10 Word</t>
-  </si>
-  <si>
-    <t>Top 10 Word Count</t>
-  </si>
-  <si>
     <t xml:space="preserve">really </t>
   </si>
   <si>
     <t>Total</t>
   </si>
   <si>
-    <t>S1 Eps</t>
-  </si>
-  <si>
-    <t>S2 Eps</t>
-  </si>
-  <si>
-    <t>S3 Eps</t>
-  </si>
-  <si>
-    <t>S4 Eps</t>
-  </si>
-  <si>
-    <t>S5 Eps</t>
-  </si>
-  <si>
-    <t>S6 Eps</t>
-  </si>
-  <si>
     <t>oh my god</t>
   </si>
   <si>
@@ -323,9 +202,6 @@
     <t>aw geez</t>
   </si>
   <si>
-    <t>Total Eps</t>
-  </si>
-  <si>
     <t>S1E1</t>
   </si>
   <si>
@@ -596,9 +472,6 @@
     <t>S5E22</t>
   </si>
   <si>
-    <t>S7 Eps</t>
-  </si>
-  <si>
     <t>S6E1</t>
   </si>
   <si>
@@ -693,6 +566,132 @@
   </si>
   <si>
     <t>S7E12</t>
+  </si>
+  <si>
+    <t>S1Eps</t>
+  </si>
+  <si>
+    <t>S1Lines</t>
+  </si>
+  <si>
+    <t>S2Eps</t>
+  </si>
+  <si>
+    <t>S2Lines</t>
+  </si>
+  <si>
+    <t>S3Eps</t>
+  </si>
+  <si>
+    <t>S3Lines</t>
+  </si>
+  <si>
+    <t>S4Eps</t>
+  </si>
+  <si>
+    <t>S4Lines</t>
+  </si>
+  <si>
+    <t>S5Eps</t>
+  </si>
+  <si>
+    <t>S5Lines</t>
+  </si>
+  <si>
+    <t>S6Eps</t>
+  </si>
+  <si>
+    <t>S6Lines</t>
+  </si>
+  <si>
+    <t>S7Eps</t>
+  </si>
+  <si>
+    <t>S7Lines</t>
+  </si>
+  <si>
+    <t>TotalEps</t>
+  </si>
+  <si>
+    <t>TotalLines</t>
+  </si>
+  <si>
+    <t>Top1Line</t>
+  </si>
+  <si>
+    <t>Top1LineCount</t>
+  </si>
+  <si>
+    <t>Top2Line</t>
+  </si>
+  <si>
+    <t>Top2LineCount</t>
+  </si>
+  <si>
+    <t>Top3Line</t>
+  </si>
+  <si>
+    <t>Top3LineCount</t>
+  </si>
+  <si>
+    <t>Top1Word</t>
+  </si>
+  <si>
+    <t>Top1WordCount</t>
+  </si>
+  <si>
+    <t>Top2Word</t>
+  </si>
+  <si>
+    <t>Top2WordCount</t>
+  </si>
+  <si>
+    <t>Top3Word</t>
+  </si>
+  <si>
+    <t>Top3WordCount</t>
+  </si>
+  <si>
+    <t>Top4Word</t>
+  </si>
+  <si>
+    <t>Top4WordCount</t>
+  </si>
+  <si>
+    <t>Top5Word</t>
+  </si>
+  <si>
+    <t>Top5WordCount</t>
+  </si>
+  <si>
+    <t>Top6Word</t>
+  </si>
+  <si>
+    <t>Top6WordCount</t>
+  </si>
+  <si>
+    <t>Top7Word</t>
+  </si>
+  <si>
+    <t>Top7WordCount</t>
+  </si>
+  <si>
+    <t>Top8Word</t>
+  </si>
+  <si>
+    <t>Top8WordCount</t>
+  </si>
+  <si>
+    <t>Top9Word</t>
+  </si>
+  <si>
+    <t>Top9WordCount</t>
+  </si>
+  <si>
+    <t>Top10Word</t>
+  </si>
+  <si>
+    <t>Top10WordCount</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DDB9F8-86F9-9B4F-98A2-943E1E9471F1}">
   <dimension ref="A1:FI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="ER1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="FM16" sqref="FM16"/>
+    <sheetView tabSelected="1" topLeftCell="EZ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="FK16" sqref="FK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1110,496 +1109,496 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W1" t="s">
+        <v>72</v>
+      </c>
+      <c r="X1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="AD1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW1" t="s">
         <v>96</v>
       </c>
-      <c r="E1" t="s">
+      <c r="AX1" t="s">
         <v>97</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AY1" t="s">
         <v>98</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AZ1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="BA1" t="s">
         <v>100</v>
       </c>
-      <c r="I1" t="s">
+      <c r="BB1" t="s">
+        <v>183</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>184</v>
+      </c>
+      <c r="BD1" t="s">
         <v>101</v>
       </c>
-      <c r="J1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="BE1" t="s">
         <v>102</v>
       </c>
-      <c r="M1" t="s">
+      <c r="BF1" t="s">
         <v>103</v>
       </c>
-      <c r="N1" t="s">
+      <c r="BG1" t="s">
         <v>104</v>
       </c>
-      <c r="O1" t="s">
+      <c r="BH1" t="s">
         <v>105</v>
       </c>
-      <c r="P1" t="s">
+      <c r="BI1" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="BJ1" t="s">
         <v>107</v>
       </c>
-      <c r="R1" t="s">
+      <c r="BK1" t="s">
         <v>108</v>
       </c>
-      <c r="S1" t="s">
+      <c r="BL1" t="s">
         <v>109</v>
       </c>
-      <c r="T1" t="s">
+      <c r="BM1" t="s">
         <v>110</v>
       </c>
-      <c r="U1" t="s">
+      <c r="BN1" t="s">
         <v>111</v>
       </c>
-      <c r="V1" t="s">
+      <c r="BO1" t="s">
         <v>112</v>
       </c>
-      <c r="W1" t="s">
+      <c r="BP1" t="s">
         <v>113</v>
       </c>
-      <c r="X1" t="s">
+      <c r="BQ1" t="s">
         <v>114</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="BR1" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="BS1" t="s">
         <v>116</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="BT1" t="s">
         <v>117</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="BU1" t="s">
         <v>118</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="BV1" t="s">
         <v>119</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="BW1" t="s">
         <v>120</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="BX1" t="s">
         <v>121</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="BY1" t="s">
         <v>122</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="BZ1" t="s">
+        <v>185</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>186</v>
+      </c>
+      <c r="CB1" t="s">
         <v>123</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="CC1" t="s">
         <v>124</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="CD1" t="s">
         <v>125</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="CE1" t="s">
         <v>126</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="CF1" t="s">
         <v>127</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="CG1" t="s">
         <v>128</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="CH1" t="s">
         <v>129</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="CI1" t="s">
         <v>130</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="CJ1" t="s">
         <v>131</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="CK1" t="s">
         <v>132</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="CL1" t="s">
         <v>133</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="CM1" t="s">
         <v>134</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="CN1" t="s">
         <v>135</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="CO1" t="s">
         <v>136</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="CP1" t="s">
         <v>137</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="CQ1" t="s">
         <v>138</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="CR1" t="s">
         <v>139</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="CS1" t="s">
         <v>140</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="CT1" t="s">
         <v>141</v>
       </c>
-      <c r="BB1" t="s">
-        <v>81</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>15</v>
-      </c>
-      <c r="BD1" t="s">
+      <c r="CU1" t="s">
         <v>142</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="CV1" t="s">
         <v>143</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="CW1" t="s">
         <v>144</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="CX1" t="s">
+        <v>187</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>188</v>
+      </c>
+      <c r="CZ1" t="s">
         <v>145</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="DA1" t="s">
         <v>146</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="DB1" t="s">
         <v>147</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="DC1" t="s">
         <v>148</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="DD1" t="s">
         <v>149</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="DE1" t="s">
         <v>150</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="DF1" t="s">
         <v>151</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="DG1" t="s">
         <v>152</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="DH1" t="s">
         <v>153</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="DI1" t="s">
         <v>154</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="DJ1" t="s">
         <v>155</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="DK1" t="s">
         <v>156</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="DL1" t="s">
         <v>157</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="DM1" t="s">
         <v>158</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="DN1" t="s">
         <v>159</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="DO1" t="s">
         <v>160</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="DP1" t="s">
         <v>161</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="DQ1" t="s">
         <v>162</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="DR1" t="s">
         <v>163</v>
       </c>
-      <c r="BZ1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>16</v>
-      </c>
-      <c r="CB1" t="s">
+      <c r="DS1" t="s">
         <v>164</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="DT1" t="s">
+        <v>189</v>
+      </c>
+      <c r="DU1" t="s">
+        <v>190</v>
+      </c>
+      <c r="DV1" t="s">
         <v>165</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="DW1" t="s">
         <v>166</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="DX1" t="s">
         <v>167</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="DY1" t="s">
         <v>168</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="DZ1" t="s">
         <v>169</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="EA1" t="s">
         <v>170</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="EB1" t="s">
         <v>171</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="EC1" t="s">
         <v>172</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="ED1" t="s">
         <v>173</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="EE1" t="s">
         <v>174</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="EF1" t="s">
         <v>175</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="EG1" t="s">
         <v>176</v>
       </c>
-      <c r="CO1" t="s">
-        <v>177</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>178</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>179</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>180</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>181</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>182</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>183</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>184</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>185</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>83</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>17</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>187</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>188</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>189</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>190</v>
-      </c>
-      <c r="DD1" t="s">
+      <c r="EH1" t="s">
         <v>191</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="EI1" t="s">
         <v>192</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="EJ1" t="s">
         <v>193</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="EK1" t="s">
         <v>194</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="EL1" t="s">
         <v>195</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="EM1" t="s">
         <v>196</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="EN1" t="s">
         <v>197</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="EO1" t="s">
         <v>198</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="EP1" t="s">
         <v>199</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="EQ1" t="s">
         <v>200</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="ER1" t="s">
         <v>201</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="ES1" t="s">
         <v>202</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="EV1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="EW1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="DT1" t="s">
-        <v>186</v>
-      </c>
-      <c r="DU1" t="s">
-        <v>18</v>
-      </c>
-      <c r="DV1" t="s">
+      <c r="EX1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="EY1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="EZ1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="FA1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="FF1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="FG1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="EH1" t="s">
-        <v>95</v>
-      </c>
-      <c r="EI1" t="s">
-        <v>11</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>19</v>
-      </c>
-      <c r="EK1" t="s">
-        <v>25</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>20</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>26</v>
-      </c>
-      <c r="EN1" t="s">
-        <v>21</v>
-      </c>
-      <c r="EO1" t="s">
-        <v>27</v>
-      </c>
-      <c r="EP1" t="s">
-        <v>22</v>
-      </c>
-      <c r="EQ1" t="s">
-        <v>59</v>
-      </c>
-      <c r="ER1" t="s">
-        <v>23</v>
-      </c>
-      <c r="ES1" t="s">
-        <v>60</v>
-      </c>
-      <c r="ET1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="EV1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="EX1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="EY1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="EZ1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="FA1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="FB1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="FC1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="FD1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="FE1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="FF1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="FG1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="FH1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="FI1" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:165" x14ac:dyDescent="0.2">
@@ -2029,79 +2028,79 @@
         <v>18087</v>
       </c>
       <c r="EJ2" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EK2">
         <v>106</v>
       </c>
       <c r="EL2" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EM2">
         <v>76</v>
       </c>
       <c r="EN2" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="EO2">
         <v>40</v>
       </c>
       <c r="EP2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="EQ2">
         <v>916</v>
       </c>
       <c r="ER2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="ES2">
         <v>889</v>
       </c>
       <c r="ET2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="EU2">
         <v>841</v>
       </c>
       <c r="EV2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="EW2">
         <v>719</v>
       </c>
       <c r="EX2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="EY2">
         <v>563</v>
       </c>
       <c r="EZ2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="FA2">
         <v>434</v>
       </c>
       <c r="FB2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="FC2">
         <v>392</v>
       </c>
       <c r="FD2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="FE2">
         <v>368</v>
       </c>
       <c r="FF2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="FG2">
         <v>368</v>
       </c>
       <c r="FH2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="FI2">
         <v>353</v>
@@ -2534,79 +2533,79 @@
         <v>6287</v>
       </c>
       <c r="EJ3" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="EK3">
         <v>18</v>
       </c>
       <c r="EL3" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EM3">
         <v>15</v>
       </c>
       <c r="EN3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="EO3">
         <v>12</v>
       </c>
       <c r="EP3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="EQ3">
         <v>311</v>
       </c>
       <c r="ER3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="ES3">
         <v>263</v>
       </c>
       <c r="ET3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="EU3">
         <v>230</v>
       </c>
       <c r="EV3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="EW3">
         <v>137</v>
       </c>
       <c r="EX3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="EY3">
         <v>133</v>
       </c>
       <c r="EZ3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="FA3">
         <v>130</v>
       </c>
       <c r="FB3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="FC3">
         <v>129</v>
       </c>
       <c r="FD3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="FE3">
         <v>123</v>
       </c>
       <c r="FF3" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="FG3">
         <v>122</v>
       </c>
       <c r="FH3" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="FI3">
         <v>111</v>
@@ -3039,79 +3038,79 @@
         <v>5375</v>
       </c>
       <c r="EJ4" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EK4">
         <v>21</v>
       </c>
       <c r="EL4" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="EM4">
         <v>20</v>
       </c>
       <c r="EN4" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EO4">
         <v>19</v>
       </c>
       <c r="EP4" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="EQ4">
         <v>255</v>
       </c>
       <c r="ER4" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="ES4">
         <v>234</v>
       </c>
       <c r="ET4" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="EU4">
         <v>214</v>
       </c>
       <c r="EV4" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="EW4">
         <v>198</v>
       </c>
       <c r="EX4" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="EY4">
         <v>175</v>
       </c>
       <c r="EZ4" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="FA4">
         <v>175</v>
       </c>
       <c r="FB4" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="FC4">
         <v>138</v>
       </c>
       <c r="FD4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="FE4">
         <v>133</v>
       </c>
       <c r="FF4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="FG4">
         <v>132</v>
       </c>
       <c r="FH4" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="FI4">
         <v>123</v>
@@ -3544,79 +3543,79 @@
         <v>5148</v>
       </c>
       <c r="EJ5" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="EK5">
         <v>35</v>
       </c>
       <c r="EL5" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EM5">
         <v>25</v>
       </c>
       <c r="EN5" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EO5">
         <v>21</v>
       </c>
       <c r="EP5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="EQ5">
         <v>350</v>
       </c>
       <c r="ER5" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="ES5">
         <v>304</v>
       </c>
       <c r="ET5" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="EU5">
         <v>263</v>
       </c>
       <c r="EV5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="EW5">
         <v>246</v>
       </c>
       <c r="EX5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="EY5">
         <v>231</v>
       </c>
       <c r="EZ5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="FA5">
         <v>221</v>
       </c>
       <c r="FB5" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="FC5">
         <v>184</v>
       </c>
       <c r="FD5" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="FE5">
         <v>167</v>
       </c>
       <c r="FF5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="FG5">
         <v>160</v>
       </c>
       <c r="FH5" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="FI5">
         <v>157</v>
@@ -4049,79 +4048,79 @@
         <v>4995</v>
       </c>
       <c r="EJ6" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EK6">
         <v>16</v>
       </c>
       <c r="EL6" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="EM6">
         <v>7</v>
       </c>
       <c r="EN6" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="EO6">
         <v>6</v>
       </c>
       <c r="EP6" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="EQ6">
         <v>244</v>
       </c>
       <c r="ER6" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="ES6">
         <v>210</v>
       </c>
       <c r="ET6" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="EU6">
         <v>175</v>
       </c>
       <c r="EV6" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="EW6">
         <v>136</v>
       </c>
       <c r="EX6" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="EY6">
         <v>121</v>
       </c>
       <c r="EZ6" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="FA6">
         <v>117</v>
       </c>
       <c r="FB6" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="FC6">
         <v>116</v>
       </c>
       <c r="FD6" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="FE6">
         <v>112</v>
       </c>
       <c r="FF6" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="FG6">
         <v>98</v>
       </c>
       <c r="FH6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="FI6">
         <v>95</v>
@@ -4554,79 +4553,79 @@
         <v>4216</v>
       </c>
       <c r="EJ7" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EK7">
         <v>35</v>
       </c>
       <c r="EL7" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EM7">
         <v>16</v>
       </c>
       <c r="EN7" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="EO7">
         <v>14</v>
       </c>
       <c r="EP7" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="EQ7">
         <v>242</v>
       </c>
       <c r="ER7" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="ES7">
         <v>233</v>
       </c>
       <c r="ET7" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="EU7">
         <v>203</v>
       </c>
       <c r="EV7" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="EW7">
         <v>203</v>
       </c>
       <c r="EX7" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="EY7">
         <v>199</v>
       </c>
       <c r="EZ7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="FA7">
         <v>157</v>
       </c>
       <c r="FB7" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="FC7">
         <v>149</v>
       </c>
       <c r="FD7" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="FE7">
         <v>142</v>
       </c>
       <c r="FF7" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="FG7">
         <v>122</v>
       </c>
       <c r="FH7" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="FI7">
         <v>116</v>
@@ -5059,79 +5058,79 @@
         <v>3627</v>
       </c>
       <c r="EJ8" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EK8">
         <v>30</v>
       </c>
       <c r="EL8" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EM8">
         <v>16</v>
       </c>
       <c r="EN8" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="EO8">
         <v>16</v>
       </c>
       <c r="EP8" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="EQ8">
         <v>183</v>
       </c>
       <c r="ER8" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="ES8">
         <v>180</v>
       </c>
       <c r="ET8" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="EU8">
         <v>168</v>
       </c>
       <c r="EV8" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="EW8">
         <v>163</v>
       </c>
       <c r="EX8" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="EY8">
         <v>148</v>
       </c>
       <c r="EZ8" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="FA8">
         <v>127</v>
       </c>
       <c r="FB8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="FC8">
         <v>120</v>
       </c>
       <c r="FD8" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="FE8">
         <v>94</v>
       </c>
       <c r="FF8" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="FG8">
         <v>86</v>
       </c>
       <c r="FH8" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="FI8">
         <v>79</v>
@@ -5564,79 +5563,79 @@
         <v>2833</v>
       </c>
       <c r="EJ9" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="EK9">
         <v>32</v>
       </c>
       <c r="EL9" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EM9">
         <v>13</v>
       </c>
       <c r="EN9" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="EO9">
         <v>8</v>
       </c>
       <c r="EP9" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="EQ9">
         <v>123</v>
       </c>
       <c r="ER9" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="ES9">
         <v>103</v>
       </c>
       <c r="ET9" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="EU9">
         <v>101</v>
       </c>
       <c r="EV9" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="EW9">
         <v>96</v>
       </c>
       <c r="EX9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="EY9">
         <v>87</v>
       </c>
       <c r="EZ9" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="FA9">
         <v>86</v>
       </c>
       <c r="FB9" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="FC9">
         <v>83</v>
       </c>
       <c r="FD9" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="FE9">
         <v>81</v>
       </c>
       <c r="FF9" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="FG9">
         <v>78</v>
       </c>
       <c r="FH9" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="FI9">
         <v>67</v>
@@ -6069,79 +6068,79 @@
         <v>1327</v>
       </c>
       <c r="EJ10" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EK10">
         <v>8</v>
       </c>
       <c r="EL10" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="EM10">
         <v>8</v>
       </c>
       <c r="EN10" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="EO10">
         <v>4</v>
       </c>
       <c r="EP10" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="EQ10">
         <v>69</v>
       </c>
       <c r="ER10" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="ES10">
         <v>50</v>
       </c>
       <c r="ET10" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="EU10">
         <v>48</v>
       </c>
       <c r="EV10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="EW10">
         <v>48</v>
       </c>
       <c r="EX10" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="EY10">
         <v>48</v>
       </c>
       <c r="EZ10" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="FA10">
         <v>43</v>
       </c>
       <c r="FB10" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="FC10">
         <v>40</v>
       </c>
       <c r="FD10" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="FE10">
         <v>38</v>
       </c>
       <c r="FF10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="FG10">
         <v>38</v>
       </c>
       <c r="FH10" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="FI10">
         <v>32</v>
@@ -6574,79 +6573,79 @@
         <v>1325</v>
       </c>
       <c r="EJ11" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="EK11">
         <v>9</v>
       </c>
       <c r="EL11" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="EM11">
         <v>8</v>
       </c>
       <c r="EN11" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="EO11">
         <v>7</v>
       </c>
       <c r="EP11" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="EQ11">
         <v>104</v>
       </c>
       <c r="ER11" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="ES11">
         <v>72</v>
       </c>
       <c r="ET11" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="EU11">
         <v>70</v>
       </c>
       <c r="EV11" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="EW11">
         <v>66</v>
       </c>
       <c r="EX11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="EY11">
         <v>66</v>
       </c>
       <c r="EZ11" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="FA11">
         <v>63</v>
       </c>
       <c r="FB11" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="FC11">
         <v>44</v>
       </c>
       <c r="FD11" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="FE11">
         <v>41</v>
       </c>
       <c r="FF11" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="FG11">
         <v>35</v>
       </c>
       <c r="FH11" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="FI11">
         <v>33</v>
@@ -6654,7 +6653,7 @@
     </row>
     <row r="12" spans="1:165" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>6</v>

</xml_diff>

<commit_message>
added d3 reference and added formatting for integers
</commit_message>
<xml_diff>
--- a/data/all_data.xlsx
+++ b/data/all_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troyspringmeadows/tv-time/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6182D2-92A8-8E46-9EDF-3997C3002FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C44B6D-6460-3A4B-9D83-8C2660506FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32680" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{D6E1F5BB-695F-B243-9E7C-4B6C1748E0AB}"/>
+    <workbookView xWindow="-33920" yWindow="1400" windowWidth="28800" windowHeight="16520" xr2:uid="{D6E1F5BB-695F-B243-9E7C-4B6C1748E0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,372 +202,6 @@
     <t>aw geez</t>
   </si>
   <si>
-    <t>S1E1</t>
-  </si>
-  <si>
-    <t>S1E2</t>
-  </si>
-  <si>
-    <t>S1E3</t>
-  </si>
-  <si>
-    <t>S1E4</t>
-  </si>
-  <si>
-    <t>S1E5</t>
-  </si>
-  <si>
-    <t>S1E6</t>
-  </si>
-  <si>
-    <t>S2E1</t>
-  </si>
-  <si>
-    <t>S2E2</t>
-  </si>
-  <si>
-    <t>S2E3</t>
-  </si>
-  <si>
-    <t>S2E4</t>
-  </si>
-  <si>
-    <t>S2E5</t>
-  </si>
-  <si>
-    <t>S2E6</t>
-  </si>
-  <si>
-    <t>S2E7</t>
-  </si>
-  <si>
-    <t>S2E8</t>
-  </si>
-  <si>
-    <t>S2E9</t>
-  </si>
-  <si>
-    <t>S2E10</t>
-  </si>
-  <si>
-    <t>S2E11</t>
-  </si>
-  <si>
-    <t>S2E12</t>
-  </si>
-  <si>
-    <t>S2E13</t>
-  </si>
-  <si>
-    <t>S2E14</t>
-  </si>
-  <si>
-    <t>S2E15</t>
-  </si>
-  <si>
-    <t>S2E16</t>
-  </si>
-  <si>
-    <t>S2E17</t>
-  </si>
-  <si>
-    <t>S2E18</t>
-  </si>
-  <si>
-    <t>S2E19</t>
-  </si>
-  <si>
-    <t>S2E20</t>
-  </si>
-  <si>
-    <t>S2E21</t>
-  </si>
-  <si>
-    <t>S2E22</t>
-  </si>
-  <si>
-    <t>S2E23</t>
-  </si>
-  <si>
-    <t>S2E24</t>
-  </si>
-  <si>
-    <t>S3E1</t>
-  </si>
-  <si>
-    <t>S3E2</t>
-  </si>
-  <si>
-    <t>S3E3</t>
-  </si>
-  <si>
-    <t>S3E4</t>
-  </si>
-  <si>
-    <t>S3E5</t>
-  </si>
-  <si>
-    <t>S3E6</t>
-  </si>
-  <si>
-    <t>S3E7</t>
-  </si>
-  <si>
-    <t>S3E8</t>
-  </si>
-  <si>
-    <t>S3E9</t>
-  </si>
-  <si>
-    <t>S3E10</t>
-  </si>
-  <si>
-    <t>S3E11</t>
-  </si>
-  <si>
-    <t>S3E12</t>
-  </si>
-  <si>
-    <t>S3E13</t>
-  </si>
-  <si>
-    <t>S3E14</t>
-  </si>
-  <si>
-    <t>S3E15</t>
-  </si>
-  <si>
-    <t>S3E16</t>
-  </si>
-  <si>
-    <t>S4E1</t>
-  </si>
-  <si>
-    <t>S4E2</t>
-  </si>
-  <si>
-    <t>S4E3</t>
-  </si>
-  <si>
-    <t>S4E4</t>
-  </si>
-  <si>
-    <t>S4E5</t>
-  </si>
-  <si>
-    <t>S4E6</t>
-  </si>
-  <si>
-    <t>S4E7</t>
-  </si>
-  <si>
-    <t>S4E8</t>
-  </si>
-  <si>
-    <t>S4E9</t>
-  </si>
-  <si>
-    <t>S4E10</t>
-  </si>
-  <si>
-    <t>S4E11</t>
-  </si>
-  <si>
-    <t>S4E12</t>
-  </si>
-  <si>
-    <t>S4E13</t>
-  </si>
-  <si>
-    <t>S4E14</t>
-  </si>
-  <si>
-    <t>S4E15</t>
-  </si>
-  <si>
-    <t>S4E16</t>
-  </si>
-  <si>
-    <t>S4E17</t>
-  </si>
-  <si>
-    <t>S4E18</t>
-  </si>
-  <si>
-    <t>S4E19</t>
-  </si>
-  <si>
-    <t>S4E20</t>
-  </si>
-  <si>
-    <t>S4E21</t>
-  </si>
-  <si>
-    <t>S4E22</t>
-  </si>
-  <si>
-    <t>S5E1</t>
-  </si>
-  <si>
-    <t>S5E2</t>
-  </si>
-  <si>
-    <t>S5E3</t>
-  </si>
-  <si>
-    <t>S5E4</t>
-  </si>
-  <si>
-    <t>S5E5</t>
-  </si>
-  <si>
-    <t>S5E6</t>
-  </si>
-  <si>
-    <t>S5E7</t>
-  </si>
-  <si>
-    <t>S5E8</t>
-  </si>
-  <si>
-    <t>S5E9</t>
-  </si>
-  <si>
-    <t>S5E10</t>
-  </si>
-  <si>
-    <t>S5E11</t>
-  </si>
-  <si>
-    <t>S5E12</t>
-  </si>
-  <si>
-    <t>S5E13</t>
-  </si>
-  <si>
-    <t>S5E14</t>
-  </si>
-  <si>
-    <t>S5E15</t>
-  </si>
-  <si>
-    <t>S5E16</t>
-  </si>
-  <si>
-    <t>S5E17</t>
-  </si>
-  <si>
-    <t>S5E18</t>
-  </si>
-  <si>
-    <t>S5E19</t>
-  </si>
-  <si>
-    <t>S5E20</t>
-  </si>
-  <si>
-    <t>S5E21</t>
-  </si>
-  <si>
-    <t>S5E22</t>
-  </si>
-  <si>
-    <t>S6E1</t>
-  </si>
-  <si>
-    <t>S6E2</t>
-  </si>
-  <si>
-    <t>S6E3</t>
-  </si>
-  <si>
-    <t>S6E4</t>
-  </si>
-  <si>
-    <t>S6E5</t>
-  </si>
-  <si>
-    <t>S6E6</t>
-  </si>
-  <si>
-    <t>S6E7</t>
-  </si>
-  <si>
-    <t>S6E8</t>
-  </si>
-  <si>
-    <t>S6E9</t>
-  </si>
-  <si>
-    <t>S6E10</t>
-  </si>
-  <si>
-    <t>S6E11</t>
-  </si>
-  <si>
-    <t>S6E12</t>
-  </si>
-  <si>
-    <t>S6E13</t>
-  </si>
-  <si>
-    <t>S6E14</t>
-  </si>
-  <si>
-    <t>S6E15</t>
-  </si>
-  <si>
-    <t>S6E16</t>
-  </si>
-  <si>
-    <t>S6E17</t>
-  </si>
-  <si>
-    <t>S6E18</t>
-  </si>
-  <si>
-    <t>S6E19</t>
-  </si>
-  <si>
-    <t>S6E20</t>
-  </si>
-  <si>
-    <t>S7E1</t>
-  </si>
-  <si>
-    <t>S7E2</t>
-  </si>
-  <si>
-    <t>S7E3</t>
-  </si>
-  <si>
-    <t>S7E4</t>
-  </si>
-  <si>
-    <t>S7E5</t>
-  </si>
-  <si>
-    <t>S7E6</t>
-  </si>
-  <si>
-    <t>S7E7</t>
-  </si>
-  <si>
-    <t>S7E8</t>
-  </si>
-  <si>
-    <t>S7E9</t>
-  </si>
-  <si>
-    <t>S7E10</t>
-  </si>
-  <si>
-    <t>S7E11</t>
-  </si>
-  <si>
-    <t>S7E12</t>
-  </si>
-  <si>
     <t>S1Eps</t>
   </si>
   <si>
@@ -692,6 +326,372 @@
   </si>
   <si>
     <t>Top10WordCount</t>
+  </si>
+  <si>
+    <t>s1e1</t>
+  </si>
+  <si>
+    <t>s1e2</t>
+  </si>
+  <si>
+    <t>s1e3</t>
+  </si>
+  <si>
+    <t>s1e4</t>
+  </si>
+  <si>
+    <t>s1e5</t>
+  </si>
+  <si>
+    <t>s1e6</t>
+  </si>
+  <si>
+    <t>s2e1</t>
+  </si>
+  <si>
+    <t>s2e2</t>
+  </si>
+  <si>
+    <t>s2e3</t>
+  </si>
+  <si>
+    <t>s2e4</t>
+  </si>
+  <si>
+    <t>s2e5</t>
+  </si>
+  <si>
+    <t>s2e6</t>
+  </si>
+  <si>
+    <t>s2e7</t>
+  </si>
+  <si>
+    <t>s2e8</t>
+  </si>
+  <si>
+    <t>s2e9</t>
+  </si>
+  <si>
+    <t>s2e10</t>
+  </si>
+  <si>
+    <t>s2e11</t>
+  </si>
+  <si>
+    <t>s2e12</t>
+  </si>
+  <si>
+    <t>s2e13</t>
+  </si>
+  <si>
+    <t>s2e14</t>
+  </si>
+  <si>
+    <t>s2e15</t>
+  </si>
+  <si>
+    <t>s2e16</t>
+  </si>
+  <si>
+    <t>s2e17</t>
+  </si>
+  <si>
+    <t>s2e18</t>
+  </si>
+  <si>
+    <t>s2e19</t>
+  </si>
+  <si>
+    <t>s2e20</t>
+  </si>
+  <si>
+    <t>s2e21</t>
+  </si>
+  <si>
+    <t>s2e22</t>
+  </si>
+  <si>
+    <t>s2e23</t>
+  </si>
+  <si>
+    <t>s2e24</t>
+  </si>
+  <si>
+    <t>s3e1</t>
+  </si>
+  <si>
+    <t>s3e2</t>
+  </si>
+  <si>
+    <t>s3e3</t>
+  </si>
+  <si>
+    <t>s3e4</t>
+  </si>
+  <si>
+    <t>s3e5</t>
+  </si>
+  <si>
+    <t>s3e6</t>
+  </si>
+  <si>
+    <t>s3e7</t>
+  </si>
+  <si>
+    <t>s3e8</t>
+  </si>
+  <si>
+    <t>s3e9</t>
+  </si>
+  <si>
+    <t>s3e10</t>
+  </si>
+  <si>
+    <t>s3e11</t>
+  </si>
+  <si>
+    <t>s3e12</t>
+  </si>
+  <si>
+    <t>s3e13</t>
+  </si>
+  <si>
+    <t>s3e14</t>
+  </si>
+  <si>
+    <t>s3e15</t>
+  </si>
+  <si>
+    <t>s3e16</t>
+  </si>
+  <si>
+    <t>s4e1</t>
+  </si>
+  <si>
+    <t>s4e2</t>
+  </si>
+  <si>
+    <t>s4e3</t>
+  </si>
+  <si>
+    <t>s4e4</t>
+  </si>
+  <si>
+    <t>s4e5</t>
+  </si>
+  <si>
+    <t>s4e6</t>
+  </si>
+  <si>
+    <t>s4e7</t>
+  </si>
+  <si>
+    <t>s4e8</t>
+  </si>
+  <si>
+    <t>s4e9</t>
+  </si>
+  <si>
+    <t>s4e10</t>
+  </si>
+  <si>
+    <t>s4e11</t>
+  </si>
+  <si>
+    <t>s4e12</t>
+  </si>
+  <si>
+    <t>s4e13</t>
+  </si>
+  <si>
+    <t>s4e14</t>
+  </si>
+  <si>
+    <t>s4e15</t>
+  </si>
+  <si>
+    <t>s4e16</t>
+  </si>
+  <si>
+    <t>s4e17</t>
+  </si>
+  <si>
+    <t>s4e18</t>
+  </si>
+  <si>
+    <t>s4e19</t>
+  </si>
+  <si>
+    <t>s4e20</t>
+  </si>
+  <si>
+    <t>s4e21</t>
+  </si>
+  <si>
+    <t>s4e22</t>
+  </si>
+  <si>
+    <t>s5e1</t>
+  </si>
+  <si>
+    <t>s5e2</t>
+  </si>
+  <si>
+    <t>s5e3</t>
+  </si>
+  <si>
+    <t>s5e4</t>
+  </si>
+  <si>
+    <t>s5e5</t>
+  </si>
+  <si>
+    <t>s5e6</t>
+  </si>
+  <si>
+    <t>s5e7</t>
+  </si>
+  <si>
+    <t>s5e8</t>
+  </si>
+  <si>
+    <t>s5e9</t>
+  </si>
+  <si>
+    <t>s5e10</t>
+  </si>
+  <si>
+    <t>s5e11</t>
+  </si>
+  <si>
+    <t>s5e12</t>
+  </si>
+  <si>
+    <t>s5e13</t>
+  </si>
+  <si>
+    <t>s5e14</t>
+  </si>
+  <si>
+    <t>s5e15</t>
+  </si>
+  <si>
+    <t>s5e16</t>
+  </si>
+  <si>
+    <t>s5e17</t>
+  </si>
+  <si>
+    <t>s5e18</t>
+  </si>
+  <si>
+    <t>s5e19</t>
+  </si>
+  <si>
+    <t>s5e20</t>
+  </si>
+  <si>
+    <t>s5e21</t>
+  </si>
+  <si>
+    <t>s5e22</t>
+  </si>
+  <si>
+    <t>s6e1</t>
+  </si>
+  <si>
+    <t>s6e2</t>
+  </si>
+  <si>
+    <t>s6e3</t>
+  </si>
+  <si>
+    <t>s6e4</t>
+  </si>
+  <si>
+    <t>s6e5</t>
+  </si>
+  <si>
+    <t>s6e6</t>
+  </si>
+  <si>
+    <t>s6e7</t>
+  </si>
+  <si>
+    <t>s6e8</t>
+  </si>
+  <si>
+    <t>s6e9</t>
+  </si>
+  <si>
+    <t>s6e10</t>
+  </si>
+  <si>
+    <t>s6e11</t>
+  </si>
+  <si>
+    <t>s6e12</t>
+  </si>
+  <si>
+    <t>s6e13</t>
+  </si>
+  <si>
+    <t>s6e14</t>
+  </si>
+  <si>
+    <t>s6e15</t>
+  </si>
+  <si>
+    <t>s6e16</t>
+  </si>
+  <si>
+    <t>s6e17</t>
+  </si>
+  <si>
+    <t>s6e18</t>
+  </si>
+  <si>
+    <t>s6e19</t>
+  </si>
+  <si>
+    <t>s6e20</t>
+  </si>
+  <si>
+    <t>s7e1</t>
+  </si>
+  <si>
+    <t>s7e2</t>
+  </si>
+  <si>
+    <t>s7e3</t>
+  </si>
+  <si>
+    <t>s7e4</t>
+  </si>
+  <si>
+    <t>s7e5</t>
+  </si>
+  <si>
+    <t>s7e6</t>
+  </si>
+  <si>
+    <t>s7e7</t>
+  </si>
+  <si>
+    <t>s7e8</t>
+  </si>
+  <si>
+    <t>s7e9</t>
+  </si>
+  <si>
+    <t>s7e10</t>
+  </si>
+  <si>
+    <t>s7e11</t>
+  </si>
+  <si>
+    <t>s7e12</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DDB9F8-86F9-9B4F-98A2-943E1E9471F1}">
   <dimension ref="A1:FI12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EZ1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="FK16" sqref="FK16"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="EI1" sqref="B1:EI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1109,496 +1109,496 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" t="s">
+        <v>106</v>
+      </c>
+      <c r="P1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>108</v>
+      </c>
+      <c r="R1" t="s">
+        <v>109</v>
+      </c>
+      <c r="S1" t="s">
+        <v>110</v>
+      </c>
+      <c r="T1" t="s">
+        <v>111</v>
+      </c>
+      <c r="U1" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" t="s">
+        <v>113</v>
+      </c>
+      <c r="W1" t="s">
+        <v>114</v>
+      </c>
+      <c r="X1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>141</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>143</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>144</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>145</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>146</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>147</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>149</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>150</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>151</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>152</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>153</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>157</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>158</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>160</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>161</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>162</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>163</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>164</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>63</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>64</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>165</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>166</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>167</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>168</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>169</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>170</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>171</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>172</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>173</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>174</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>175</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>176</v>
+      </c>
+      <c r="CN1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" t="s">
+      <c r="CO1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="CP1" t="s">
         <v>179</v>
       </c>
-      <c r="K1" t="s">
+      <c r="CQ1" t="s">
         <v>180</v>
       </c>
-      <c r="L1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="CR1" t="s">
+        <v>181</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>182</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>183</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>184</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>185</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>186</v>
+      </c>
+      <c r="CX1" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="CY1" t="s">
         <v>66</v>
       </c>
-      <c r="R1" t="s">
+      <c r="CZ1" t="s">
+        <v>187</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>188</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>189</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>190</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>191</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>192</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>193</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>194</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>195</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>196</v>
+      </c>
+      <c r="DJ1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DK1" t="s">
+        <v>198</v>
+      </c>
+      <c r="DL1" t="s">
+        <v>199</v>
+      </c>
+      <c r="DM1" t="s">
+        <v>200</v>
+      </c>
+      <c r="DN1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DO1" t="s">
+        <v>202</v>
+      </c>
+      <c r="DP1" t="s">
+        <v>203</v>
+      </c>
+      <c r="DQ1" t="s">
+        <v>204</v>
+      </c>
+      <c r="DR1" t="s">
+        <v>205</v>
+      </c>
+      <c r="DS1" t="s">
+        <v>206</v>
+      </c>
+      <c r="DT1" t="s">
         <v>67</v>
       </c>
-      <c r="S1" t="s">
+      <c r="DU1" t="s">
         <v>68</v>
       </c>
-      <c r="T1" t="s">
+      <c r="DV1" t="s">
+        <v>207</v>
+      </c>
+      <c r="DW1" t="s">
+        <v>208</v>
+      </c>
+      <c r="DX1" t="s">
+        <v>209</v>
+      </c>
+      <c r="DY1" t="s">
+        <v>210</v>
+      </c>
+      <c r="DZ1" t="s">
+        <v>211</v>
+      </c>
+      <c r="EA1" t="s">
+        <v>212</v>
+      </c>
+      <c r="EB1" t="s">
+        <v>213</v>
+      </c>
+      <c r="EC1" t="s">
+        <v>214</v>
+      </c>
+      <c r="ED1" t="s">
+        <v>215</v>
+      </c>
+      <c r="EE1" t="s">
+        <v>216</v>
+      </c>
+      <c r="EF1" t="s">
+        <v>217</v>
+      </c>
+      <c r="EG1" t="s">
+        <v>218</v>
+      </c>
+      <c r="EH1" t="s">
         <v>69</v>
       </c>
-      <c r="U1" t="s">
+      <c r="EI1" t="s">
         <v>70</v>
       </c>
-      <c r="V1" t="s">
+      <c r="EJ1" t="s">
         <v>71</v>
       </c>
-      <c r="W1" t="s">
+      <c r="EK1" t="s">
         <v>72</v>
       </c>
-      <c r="X1" t="s">
+      <c r="EL1" t="s">
         <v>73</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="EM1" t="s">
         <v>74</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="EN1" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="EO1" t="s">
         <v>76</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="EP1" t="s">
         <v>77</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="EQ1" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="ER1" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="ES1" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="ET1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="EV1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="EW1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AL1" t="s">
+      <c r="EX1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="EY1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="EZ1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="FA1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="FE1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="FF1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="FG1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="FH1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="FI1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>99</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>100</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>183</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>184</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>102</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>115</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>117</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>118</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>120</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>185</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>186</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>123</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>124</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>125</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>126</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>127</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>128</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>129</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>130</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>131</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>132</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>133</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>134</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>135</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>136</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>137</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>138</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>139</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>140</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>141</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>142</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>143</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>144</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>187</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>188</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>145</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>146</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>147</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>148</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>149</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>150</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>151</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>152</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>153</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>154</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>155</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>156</v>
-      </c>
-      <c r="DL1" t="s">
-        <v>157</v>
-      </c>
-      <c r="DM1" t="s">
-        <v>158</v>
-      </c>
-      <c r="DN1" t="s">
-        <v>159</v>
-      </c>
-      <c r="DO1" t="s">
-        <v>160</v>
-      </c>
-      <c r="DP1" t="s">
-        <v>161</v>
-      </c>
-      <c r="DQ1" t="s">
-        <v>162</v>
-      </c>
-      <c r="DR1" t="s">
-        <v>163</v>
-      </c>
-      <c r="DS1" t="s">
-        <v>164</v>
-      </c>
-      <c r="DT1" t="s">
-        <v>189</v>
-      </c>
-      <c r="DU1" t="s">
-        <v>190</v>
-      </c>
-      <c r="DV1" t="s">
-        <v>165</v>
-      </c>
-      <c r="DW1" t="s">
-        <v>166</v>
-      </c>
-      <c r="DX1" t="s">
-        <v>167</v>
-      </c>
-      <c r="DY1" t="s">
-        <v>168</v>
-      </c>
-      <c r="DZ1" t="s">
-        <v>169</v>
-      </c>
-      <c r="EA1" t="s">
-        <v>170</v>
-      </c>
-      <c r="EB1" t="s">
-        <v>171</v>
-      </c>
-      <c r="EC1" t="s">
-        <v>172</v>
-      </c>
-      <c r="ED1" t="s">
-        <v>173</v>
-      </c>
-      <c r="EE1" t="s">
-        <v>174</v>
-      </c>
-      <c r="EF1" t="s">
-        <v>175</v>
-      </c>
-      <c r="EG1" t="s">
-        <v>176</v>
-      </c>
-      <c r="EH1" t="s">
-        <v>191</v>
-      </c>
-      <c r="EI1" t="s">
-        <v>192</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>193</v>
-      </c>
-      <c r="EK1" t="s">
-        <v>194</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>195</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>196</v>
-      </c>
-      <c r="EN1" t="s">
-        <v>197</v>
-      </c>
-      <c r="EO1" t="s">
-        <v>198</v>
-      </c>
-      <c r="EP1" t="s">
-        <v>199</v>
-      </c>
-      <c r="EQ1" t="s">
-        <v>200</v>
-      </c>
-      <c r="ER1" t="s">
-        <v>201</v>
-      </c>
-      <c r="ES1" t="s">
-        <v>202</v>
-      </c>
-      <c r="ET1" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="EV1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="EX1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="EY1" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="EZ1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="FA1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="FB1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="FC1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="FD1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="FE1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="FF1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="FG1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="FH1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="FI1" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:165" x14ac:dyDescent="0.2">

</xml_diff>